<commit_message>
added bow_flag and working on fix initial design
</commit_message>
<xml_diff>
--- a/cui/data/components_lists/hull_list.xlsx
+++ b/cui/data/components_lists/hull_list.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>hull_id</t>
     <phoneticPr fontId="1"/>
@@ -102,6 +102,10 @@
   </si>
   <si>
     <t>EHP4 (full)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>With bow</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -521,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -533,7 +537,7 @@
     <col min="17" max="21" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -597,8 +601,11 @@
       <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -662,10 +669,76 @@
       <c r="U2" s="1">
         <v>9.6259999999999994</v>
       </c>
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>333</v>
+      </c>
+      <c r="C3" s="1">
+        <v>324</v>
+      </c>
+      <c r="D3" s="1">
+        <v>341610</v>
+      </c>
+      <c r="E3" s="1">
+        <v>300610</v>
+      </c>
+      <c r="F3" s="1">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1">
+        <v>20.529</v>
+      </c>
+      <c r="I3" s="1">
+        <v>9.74</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.83510801999999995</v>
+      </c>
+      <c r="K3" s="1">
+        <v>27542</v>
+      </c>
+      <c r="L3" s="1">
+        <v>5387</v>
+      </c>
+      <c r="M3" s="1">
+        <v>-4640</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1445</v>
+      </c>
+      <c r="O3" s="1">
+        <v>-178</v>
+      </c>
+      <c r="P3" s="1">
+        <v>9.6470000000000002</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>5398</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-4652</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1452</v>
+      </c>
+      <c r="T3" s="1">
+        <v>-172.3</v>
+      </c>
+      <c r="U3" s="1">
+        <v>9.6259999999999994</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>